<commit_message>
Update IP - EX 18 - Funcoes logicas (e - ou) (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 18 - Funcoes logicas (e - ou) (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 18 - Funcoes logicas (e - ou) (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA770FD4-A57F-479E-8BF0-BD49A7D72771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B73B04-A7BB-46EC-94B3-FE7692AD040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -805,29 +805,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="5" fillId="3" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="3" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1367,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1553,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q76"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1693,9 @@
       <c r="B12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="19">
+        <v>9</v>
+      </c>
       <c r="N12" s="23" t="s">
         <v>10</v>
       </c>
@@ -1728,9 +1727,17 @@
       <c r="B14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="E14" s="26"/>
-      <c r="G14" s="43"/>
+      <c r="C14" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="E14" s="26" t="b">
+        <f>AND(C12&gt;=12,C14&gt;=1.5)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="43" t="str">
+        <f>IF(AND(C12&gt;=18,C14&gt;=1.5),"Pode andar no brinquedo!","Não pode andar no brinquedo!")</f>
+        <v>Não pode andar no brinquedo!</v>
+      </c>
       <c r="H14" s="44"/>
       <c r="I14" s="44"/>
       <c r="J14" s="45"/>
@@ -1779,7 +1786,9 @@
       <c r="B21" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="19">
+        <v>18</v>
+      </c>
       <c r="N21" s="24" t="s">
         <v>10</v>
       </c>
@@ -1811,9 +1820,17 @@
       <c r="B23" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="E23" s="26"/>
-      <c r="G23" s="40"/>
+      <c r="C23" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="E23" s="26" t="b">
+        <f>OR(C21&gt;18,C23&gt;1.6)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="40" t="str">
+        <f>IF(OR(C21&gt;18,C23&gt;1.6),"Ok!","Not Ok!")</f>
+        <v>Ok!</v>
+      </c>
       <c r="H23" s="41"/>
       <c r="I23" s="42"/>
       <c r="N23" s="23" t="s">
@@ -1862,12 +1879,13 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1893,10 +1911,9 @@
       <c r="D4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="55">
         <v>1000</v>
       </c>
-      <c r="F4" s="50"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1911,14 +1928,17 @@
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
+      <c r="D7" s="49" t="str">
+        <f>IF(AND(E4&gt;=1000,E4&lt;=1300),"João vai comprar!","João não vai comprar!")</f>
+        <v>João vai comprar!</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
@@ -1955,8 +1975,7 @@
       <c r="E14" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E4:F4"/>
+  <mergeCells count="1">
     <mergeCell ref="D7:F8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>